<commit_message>
working high res jezero mars
</commit_message>
<xml_diff>
--- a/validation/umwm_wind_waveheights.xlsx
+++ b/validation/umwm_wind_waveheights.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5d40ba198affbc6f/Desktop/Main/Work/Github_Repos/umwm_titan/validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="79" documentId="8_{1ECAA66D-5BF5-4A0F-8594-AA91DC5B4E12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A2E5D58C-69BF-4B80-A696-AB430EB09220}"/>
+  <xr:revisionPtr revIDLastSave="141" documentId="8_{1ECAA66D-5BF5-4A0F-8594-AA91DC5B4E12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{407A2A63-8C57-42EF-97C6-C9B70AC1C995}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="18192" windowHeight="11472" xr2:uid="{606F5AC5-7EA0-4448-AE08-6084F6885092}"/>
+    <workbookView xWindow="88095" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{606F5AC5-7EA0-4448-AE08-6084F6885092}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>u</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>umwm</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -416,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8806629-2C9F-469E-B362-0412F78F93CE}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -465,7 +468,7 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <v>1.1299999999999999E-2</v>
+        <v>7.7999999999999996E-3</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -473,10 +476,10 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>5.9136405587196302E-2</v>
+        <v>5.9304408729076302E-2</v>
       </c>
       <c r="C5">
-        <v>0.143904480651524</v>
+        <v>0.12870000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -484,10 +487,10 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0.16662134230136799</v>
+        <v>0.16711615025997101</v>
       </c>
       <c r="C6">
-        <v>0.288904690759552</v>
+        <v>0.27060000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -495,10 +498,10 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0.30079123377799899</v>
+        <v>0.30148646235465998</v>
       </c>
       <c r="C7">
-        <v>0.45508376485014701</v>
+        <v>0.43919999999999998</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -506,10 +509,10 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>0.466569364070892</v>
+        <v>0.46737498044967601</v>
       </c>
       <c r="C8">
-        <v>0.64799288561176804</v>
+        <v>0.64270000000000005</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -517,10 +520,10 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>0.665957331657409</v>
+        <v>0.66675508022308305</v>
       </c>
       <c r="C9">
-        <v>0.86559118293386295</v>
+        <v>0.874</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -528,10 +531,10 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>0.90025967359542802</v>
+        <v>0.90093064308166504</v>
       </c>
       <c r="C10">
-        <v>1.1167007638673501</v>
+        <v>1.1404000000000001</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -539,10 +542,10 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>1.1700347661971999</v>
+        <v>1.1704741716384801</v>
       </c>
       <c r="C11">
-        <v>1.3946141424354299</v>
+        <v>1.4358</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -550,10 +553,10 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>1.4746608734130799</v>
+        <v>1.4747563600540099</v>
       </c>
       <c r="C12">
-        <v>1.6900158952555</v>
+        <v>1.7547999999999999</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -561,10 +564,10 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>1.8130415678024201</v>
+        <v>1.8127077817916799</v>
       </c>
       <c r="C13">
-        <v>2.0015096555272298</v>
+        <v>2.0783</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -572,10 +575,10 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>2.1737492084503098</v>
+        <v>2.1730816364288299</v>
       </c>
       <c r="C14">
-        <v>2.3341525362234399</v>
+        <v>2.4300999999999999</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -583,10 +586,10 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>2.5764820575714098</v>
+        <v>2.57532405853271</v>
       </c>
       <c r="C15">
-        <v>2.6819525511573299</v>
+        <v>2.7881999999999998</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -594,76 +597,79 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>3.0133423805236799</v>
+        <v>3.01165771484375</v>
       </c>
       <c r="C16">
-        <v>3.0444614704839701</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>3.1825999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A17">
         <v>15</v>
       </c>
       <c r="B17">
-        <v>3.4619321823120099</v>
+        <v>3.4597053527832</v>
       </c>
       <c r="C17">
-        <v>3.4196421601501701</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>3.5966</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A18">
         <v>16</v>
       </c>
       <c r="B18">
-        <v>3.9626369476318302</v>
+        <v>3.9599518775939901</v>
       </c>
       <c r="C18">
-        <v>3.8072418117536002</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>3.9975999999999998</v>
+      </c>
+      <c r="E18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A19">
         <v>17</v>
       </c>
       <c r="B19">
-        <v>4.4575285911559996</v>
+        <v>4.4543299674987704</v>
       </c>
       <c r="C19">
-        <v>4.2068114219166901</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>4.4093</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A20">
         <v>18</v>
       </c>
       <c r="B20">
-        <v>4.9688048362731898</v>
+        <v>4.9652414321899396</v>
       </c>
       <c r="C20">
-        <v>4.6168122332400401</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>4.8737000000000004</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A21">
         <v>19</v>
       </c>
       <c r="B21">
-        <v>5.5424065589904696</v>
+        <v>5.5381946563720703</v>
       </c>
       <c r="C21">
-        <v>5.03710716872909</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>5.3090999999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A22">
         <v>20</v>
       </c>
       <c r="B22">
-        <v>6.0849585533142001</v>
+        <v>6.0803737640380797</v>
       </c>
       <c r="C22">
-        <v>5.4678138415756496</v>
+        <v>5.8125999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated model comparison plots with RMS values
</commit_message>
<xml_diff>
--- a/validation/umwm_wind_waveheights.xlsx
+++ b/validation/umwm_wind_waveheights.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5d40ba198affbc6f/Desktop/Main/Work/Github_Repos/umwm_titan/validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="141" documentId="8_{1ECAA66D-5BF5-4A0F-8594-AA91DC5B4E12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{407A2A63-8C57-42EF-97C6-C9B70AC1C995}"/>
+  <xr:revisionPtr revIDLastSave="188" documentId="8_{1ECAA66D-5BF5-4A0F-8594-AA91DC5B4E12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{07B0A5ED-A877-4E77-912B-8CE1FE8E5C98}"/>
   <bookViews>
-    <workbookView xWindow="88095" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{606F5AC5-7EA0-4448-AE08-6084F6885092}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="18192" windowHeight="11472" xr2:uid="{606F5AC5-7EA0-4448-AE08-6084F6885092}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -100,6 +100,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -422,7 +426,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -468,7 +472,7 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <v>7.7999999999999996E-3</v>
+        <v>3.0421299999999998E-2</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -476,10 +480,10 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>5.9304408729076302E-2</v>
+        <v>8.1498347222804995E-2</v>
       </c>
       <c r="C5">
-        <v>0.12870000000000001</v>
+        <v>0.14451800000000001</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -487,10 +491,10 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0.16711615025997101</v>
+        <v>0.18736366927623699</v>
       </c>
       <c r="C6">
-        <v>0.27060000000000001</v>
+        <v>0.26693800000000001</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -498,10 +502,10 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0.30148646235465998</v>
+        <v>0.319779723882675</v>
       </c>
       <c r="C7">
-        <v>0.43919999999999998</v>
+        <v>0.43732599999999999</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -509,10 +513,10 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>0.46737498044967601</v>
+        <v>0.48304304480552601</v>
       </c>
       <c r="C8">
-        <v>0.64270000000000005</v>
+        <v>0.64294499999999999</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -520,10 +524,10 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>0.66675508022308305</v>
+        <v>0.67869186401367099</v>
       </c>
       <c r="C9">
-        <v>0.874</v>
+        <v>0.87729599999999996</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -531,10 +535,10 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>0.90093064308166504</v>
+        <v>0.90832310914993197</v>
       </c>
       <c r="C10">
-        <v>1.1404000000000001</v>
+        <v>1.14096</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -542,10 +546,10 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>1.1704741716384801</v>
+        <v>1.1727869510650599</v>
       </c>
       <c r="C11">
-        <v>1.4358</v>
+        <v>1.4317200000000001</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -553,10 +557,10 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>1.4747563600540099</v>
+        <v>1.47175681591033</v>
       </c>
       <c r="C12">
-        <v>1.7547999999999999</v>
+        <v>1.7474400000000001</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -564,10 +568,10 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>1.8127077817916799</v>
+        <v>1.80442786216735</v>
       </c>
       <c r="C13">
-        <v>2.0783</v>
+        <v>2.0729600000000001</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -575,10 +579,10 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>2.1730816364288299</v>
+        <v>2.1610410213470401</v>
       </c>
       <c r="C14">
-        <v>2.4300999999999999</v>
+        <v>2.42971</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -586,10 +590,10 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>2.57532405853271</v>
+        <v>2.5583541393279998</v>
       </c>
       <c r="C15">
-        <v>2.7881999999999998</v>
+        <v>2.7871100000000002</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -597,10 +601,10 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>3.01165771484375</v>
+        <v>2.98986363410949</v>
       </c>
       <c r="C16">
-        <v>3.1825999999999999</v>
+        <v>3.1803699999999999</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -608,10 +612,10 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>3.4597053527832</v>
+        <v>3.4347374439239502</v>
       </c>
       <c r="C17">
-        <v>3.5966</v>
+        <v>3.5927699999999998</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -619,10 +623,10 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>3.9599518775939901</v>
+        <v>3.93021535873413</v>
       </c>
       <c r="C18">
-        <v>3.9975999999999998</v>
+        <v>3.9786000000000001</v>
       </c>
       <c r="E18" t="s">
         <v>3</v>
@@ -633,10 +637,10 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>4.4543299674987704</v>
+        <v>4.4217596054077104</v>
       </c>
       <c r="C19">
-        <v>4.4093</v>
+        <v>4.3825599999999998</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -644,10 +648,10 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>4.9652414321899396</v>
+        <v>4.9297094345092702</v>
       </c>
       <c r="C20">
-        <v>4.8737000000000004</v>
+        <v>4.8433299999999999</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -655,10 +659,10 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>5.5381946563720703</v>
+        <v>5.4979319572448704</v>
       </c>
       <c r="C21">
-        <v>5.3090999999999999</v>
+        <v>5.2761300000000002</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -666,10 +670,10 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>6.0803737640380797</v>
+        <v>6.0374197959899902</v>
       </c>
       <c r="C22">
-        <v>5.8125999999999998</v>
+        <v>5.77555</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
working on shoreline diffusion synthetic model
</commit_message>
<xml_diff>
--- a/validation/umwm_wind_waveheights.xlsx
+++ b/validation/umwm_wind_waveheights.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5d40ba198affbc6f/Desktop/Main/Work/Github_Repos/umwm_titan/validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="188" documentId="8_{1ECAA66D-5BF5-4A0F-8594-AA91DC5B4E12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{07B0A5ED-A877-4E77-912B-8CE1FE8E5C98}"/>
+  <xr:revisionPtr revIDLastSave="216" documentId="8_{1ECAA66D-5BF5-4A0F-8594-AA91DC5B4E12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{590B6DCA-57CD-4939-9D88-967DF9D764BD}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="18192" windowHeight="11472" xr2:uid="{606F5AC5-7EA0-4448-AE08-6084F6885092}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>u</t>
   </si>
@@ -48,6 +48,9 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>with zeroingline 437</t>
   </si>
 </sst>
 </file>
@@ -426,12 +429,12 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -441,8 +444,11 @@
       <c r="C1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <v>0</v>
       </c>
@@ -452,8 +458,11 @@
       <c r="C2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>1</v>
       </c>
@@ -463,8 +472,11 @@
       <c r="C3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>2</v>
       </c>
@@ -474,8 +486,11 @@
       <c r="C4">
         <v>3.0421299999999998E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D4">
+        <v>3.0425600000000001E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>3</v>
       </c>
@@ -485,8 +500,11 @@
       <c r="C5">
         <v>0.14451800000000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D5">
+        <v>0.14466300000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>4</v>
       </c>
@@ -496,8 +514,11 @@
       <c r="C6">
         <v>0.26693800000000001</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D6">
+        <v>0.26702199999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>5</v>
       </c>
@@ -507,8 +528,11 @@
       <c r="C7">
         <v>0.43732599999999999</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D7">
+        <v>0.43737599999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <v>6</v>
       </c>
@@ -518,8 +542,11 @@
       <c r="C8">
         <v>0.64294499999999999</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D8">
+        <v>0.64298900000000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <v>7</v>
       </c>
@@ -529,8 +556,11 @@
       <c r="C9">
         <v>0.87729599999999996</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D9">
+        <v>0.87731800000000004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
         <v>8</v>
       </c>
@@ -540,8 +570,11 @@
       <c r="C10">
         <v>1.14096</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D10">
+        <v>1.1409499999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
         <v>9</v>
       </c>
@@ -551,8 +584,11 @@
       <c r="C11">
         <v>1.4317200000000001</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D11">
+        <v>1.43167</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
         <v>10</v>
       </c>
@@ -562,8 +598,11 @@
       <c r="C12">
         <v>1.7474400000000001</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D12">
+        <v>1.7473399999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
         <v>11</v>
       </c>
@@ -573,8 +612,11 @@
       <c r="C13">
         <v>2.0729600000000001</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D13">
+        <v>2.0727799999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
         <v>12</v>
       </c>
@@ -584,8 +626,11 @@
       <c r="C14">
         <v>2.42971</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D14">
+        <v>2.4294500000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
         <v>13</v>
       </c>
@@ -595,8 +640,11 @@
       <c r="C15">
         <v>2.7871100000000002</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D15">
+        <v>2.7867500000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
         <v>14</v>
       </c>
@@ -605,6 +653,9 @@
       </c>
       <c r="C16">
         <v>3.1803699999999999</v>
+      </c>
+      <c r="D16">
+        <v>3.17991</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -617,6 +668,9 @@
       <c r="C17">
         <v>3.5927699999999998</v>
       </c>
+      <c r="D17">
+        <v>3.5922200000000002</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A18">
@@ -628,6 +682,9 @@
       <c r="C18">
         <v>3.9786000000000001</v>
       </c>
+      <c r="D18">
+        <v>3.9779399999999998</v>
+      </c>
       <c r="E18" t="s">
         <v>3</v>
       </c>
@@ -642,6 +699,9 @@
       <c r="C19">
         <v>4.3825599999999998</v>
       </c>
+      <c r="D19">
+        <v>4.3818000000000001</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A20">
@@ -653,6 +713,9 @@
       <c r="C20">
         <v>4.8433299999999999</v>
       </c>
+      <c r="D20">
+        <v>4.8424800000000001</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A21">
@@ -664,6 +727,9 @@
       <c r="C21">
         <v>5.2761300000000002</v>
       </c>
+      <c r="D21">
+        <v>5.2751700000000001</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A22">
@@ -674,6 +740,9 @@
       </c>
       <c r="C22">
         <v>5.77555</v>
+      </c>
+      <c r="D22">
+        <v>5.7745300000000004</v>
       </c>
     </row>
   </sheetData>

</xml_diff>